<commit_message>
now the field script grabs the collection devices
</commit_message>
<xml_diff>
--- a/output/blm_swampformat_Nov2020.xlsx
+++ b/output/blm_swampformat_Nov2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itlender/Projects/BLM_data_reformatter/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F423F641-D43C-F64E-8BA9-0AB21A701C92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39894B56-2343-934F-9769-37A32C8666FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -720,7 +720,7 @@
     <t>East</t>
   </si>
   <si>
-    <t>SCCWRP YSI Pro1020</t>
+    <t>YSI Pro1020</t>
   </si>
 </sst>
 </file>
@@ -4781,7 +4781,7 @@
   <dimension ref="A1:AD300"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>